<commit_message>
updates on 9/17 afternoon
slight Matlab updates;
Power calculations in part 3
</commit_message>
<xml_diff>
--- a/PS1/q2Matlab.xlsx
+++ b/PS1/q2Matlab.xlsx
@@ -70,7 +70,7 @@
     <t>u75</t>
   </si>
   <si>
-    <t>Variable</t>
+    <t>Row</t>
   </si>
 </sst>
 </file>
@@ -403,11 +403,11 @@
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -441,19 +441,19 @@
         <v>6485.5531055150177</v>
       </c>
       <c r="C2" s="1">
-        <v>1.9532230490988312E-17</v>
+        <v>94136.767261079731</v>
       </c>
       <c r="D2" s="1">
-        <v>30956446710001.23</v>
+        <v>1.4533417348056561</v>
       </c>
       <c r="E2" s="1">
-        <v>0</v>
+        <v>7.3417652731272653E-2</v>
       </c>
       <c r="F2" s="1">
-        <v>6485.5531055150177</v>
+        <v>-178022.51072620126</v>
       </c>
       <c r="G2" s="1">
-        <v>6485.5531055150177</v>
+        <v>190993.6169372313</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -464,19 +464,19 @@
         <v>1535.4824554449801</v>
       </c>
       <c r="C3" s="1">
-        <v>-1.5493415621019609E-21</v>
+        <v>13311.508560303344</v>
       </c>
       <c r="D3" s="1">
-        <v>822907988606223.5</v>
+        <v>2.4333108254003282</v>
       </c>
       <c r="E3" s="1">
-        <v>0</v>
+        <v>7.6775683394227912E-3</v>
       </c>
       <c r="F3" s="1">
-        <v>1535.4824554449801</v>
+        <v>-24555.074322749573</v>
       </c>
       <c r="G3" s="1">
-        <v>1535.4824554449801</v>
+        <v>27626.039233639534</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -487,19 +487,19 @@
         <v>-2592.3766422845752</v>
       </c>
       <c r="C4" s="1">
-        <v>1.505866371335758E-21</v>
+        <v>16581.021845903015</v>
       </c>
       <c r="D4" s="1">
-        <v>-1409239760110224.8</v>
+        <v>-3.2981227385347851</v>
       </c>
       <c r="E4" s="1">
-        <v>1</v>
+        <v>0.99947419916835667</v>
       </c>
       <c r="F4" s="1">
-        <v>-2592.3766422845752</v>
+        <v>-35091.179460254483</v>
       </c>
       <c r="G4" s="1">
-        <v>-2592.3766422845752</v>
+        <v>29906.42617568533</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -510,19 +510,19 @@
         <v>39.340521412847821</v>
       </c>
       <c r="C5" s="1">
-        <v>8.8767642481643976E-23</v>
+        <v>844.0701183206412</v>
       </c>
       <c r="D5" s="1">
-        <v>88083137200483.328</v>
+        <v>0.98319936974425448</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>0.16302238727072171</v>
       </c>
       <c r="F5" s="1">
-        <v>39.340521412847821</v>
+        <v>-1615.0369104956087</v>
       </c>
       <c r="G5" s="1">
-        <v>39.340521412847821</v>
+        <v>1693.7179533213045</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -533,19 +533,19 @@
         <v>-740.53996141695416</v>
       </c>
       <c r="C6" s="1">
-        <v>7.1071451887925535E-19</v>
+        <v>19702.836261608834</v>
       </c>
       <c r="D6" s="1">
-        <v>-18530234307659.223</v>
+        <v>-0.79286593018120477</v>
       </c>
       <c r="E6" s="1">
-        <v>1</v>
+        <v>0.78586030175176669</v>
       </c>
       <c r="F6" s="1">
-        <v>-740.53996141695416</v>
+        <v>-39358.099034170264</v>
       </c>
       <c r="G6" s="1">
-        <v>-740.53996141695416</v>
+        <v>37877.019111336362</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -556,19 +556,19 @@
         <v>60.082333940136046</v>
       </c>
       <c r="C7" s="1">
-        <v>1.8581251697094294E-21</v>
+        <v>1121.4284432509669</v>
       </c>
       <c r="D7" s="1">
-        <v>29402842473622.43</v>
+        <v>1.1301998184381536</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>0.12950110142472249</v>
       </c>
       <c r="F7" s="1">
-        <v>60.082333940136046</v>
+        <v>-2137.9174148317593</v>
       </c>
       <c r="G7" s="1">
-        <v>60.082333940136046</v>
+        <v>2258.082082712031</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -579,19 +579,19 @@
         <v>-2.985773881607065E-2</v>
       </c>
       <c r="C8" s="1">
-        <v>-1.7229598553785877E-29</v>
+        <v>2.1627850076780044</v>
       </c>
       <c r="D8" s="1">
-        <v>-151739741848767.69</v>
+        <v>-0.29122159072365578</v>
       </c>
       <c r="E8" s="1">
-        <v>1</v>
+        <v>0.61449107639369571</v>
       </c>
       <c r="F8" s="1">
-        <v>-2.985773881607065E-2</v>
+        <v>-4.2689163538649586</v>
       </c>
       <c r="G8" s="1">
-        <v>-2.985773881607065E-2</v>
+        <v>4.2092008762328179</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -602,19 +602,19 @@
         <v>0.17535467119474801</v>
       </c>
       <c r="C9" s="1">
-        <v>-3.4667660337407771E-29</v>
+        <v>2.7490412838115721</v>
       </c>
       <c r="D9" s="1">
-        <v>628253733909995.25</v>
+        <v>1.3456003236602125</v>
       </c>
       <c r="E9" s="1">
-        <v>0</v>
+        <v>8.9559094438321996E-2</v>
       </c>
       <c r="F9" s="1">
-        <v>0.17535467119474801</v>
+        <v>-5.2127662450759331</v>
       </c>
       <c r="G9" s="1">
-        <v>0.17535467119474801</v>
+        <v>5.5634755874654296</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -625,19 +625,19 @@
         <v>1316.0319716818251</v>
       </c>
       <c r="C10" s="1">
-        <v>1.7330432449291371E-20</v>
+        <v>31408.597060780608</v>
       </c>
       <c r="D10" s="1">
-        <v>210883084744167.47</v>
+        <v>0.88388936322265432</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
+        <v>0.18861714753315018</v>
       </c>
       <c r="F10" s="1">
-        <v>1316.0319716818251</v>
+        <v>-60244.818267448165</v>
       </c>
       <c r="G10" s="1">
-        <v>1316.0319716818251</v>
+        <v>62876.882210811818</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -648,19 +648,19 @@
         <v>-1167.6884001688722</v>
       </c>
       <c r="C11" s="1">
-        <v>2.7317016677133903E-21</v>
+        <v>26600.901698513131</v>
       </c>
       <c r="D11" s="1">
-        <v>-471292292668456.31</v>
+        <v>-0.92599920354961751</v>
       </c>
       <c r="E11" s="1">
-        <v>1</v>
+        <v>0.82252528389354174</v>
       </c>
       <c r="F11" s="1">
-        <v>-1167.6884001688722</v>
+        <v>-53305.455729254609</v>
       </c>
       <c r="G11" s="1">
-        <v>-1167.6884001688722</v>
+        <v>50970.078928916861</v>
       </c>
     </row>
   </sheetData>
@@ -679,11 +679,11 @@
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -717,19 +717,19 @@
         <v>6485.5531055153451</v>
       </c>
       <c r="C2" s="1">
-        <v>1.1485651727481656E-17</v>
+        <v>94136.767261024172</v>
       </c>
       <c r="D2" s="1">
-        <v>40369112680287.984</v>
+        <v>1.4533417348065871</v>
       </c>
       <c r="E2" s="1">
-        <v>0</v>
+        <v>7.3417652731143868E-2</v>
       </c>
       <c r="F2" s="1">
-        <v>6485.5531055153451</v>
+        <v>-178022.51072609203</v>
       </c>
       <c r="G2" s="1">
-        <v>6485.5531055153451</v>
+        <v>190993.61693712272</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -740,19 +740,19 @@
         <v>1535.4824554449833</v>
       </c>
       <c r="C3" s="1">
-        <v>3.4553384236896854E-21</v>
+        <v>13311.50856030318</v>
       </c>
       <c r="D3" s="1">
-        <v>551035487832584.31</v>
+        <v>2.4333108254003628</v>
       </c>
       <c r="E3" s="1">
-        <v>0</v>
+        <v>7.677568339422014E-3</v>
       </c>
       <c r="F3" s="1">
-        <v>1535.4824554449833</v>
+        <v>-24555.074322749249</v>
       </c>
       <c r="G3" s="1">
-        <v>1535.4824554449833</v>
+        <v>27626.039233639218</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -763,19 +763,19 @@
         <v>-2592.3766422845947</v>
       </c>
       <c r="C4" s="1">
-        <v>2.0209601113590331E-21</v>
+        <v>16581.021845903037</v>
       </c>
       <c r="D4" s="1">
-        <v>-1216463925513056.5</v>
+        <v>-3.298122738534806</v>
       </c>
       <c r="E4" s="1">
-        <v>1</v>
+        <v>0.99947419916835678</v>
       </c>
       <c r="F4" s="1">
-        <v>-2592.3766422845947</v>
+        <v>-35091.179460254541</v>
       </c>
       <c r="G4" s="1">
-        <v>-2592.3766422845947</v>
+        <v>29906.426175685356</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -786,19 +786,19 @@
         <v>39.340521412847934</v>
       </c>
       <c r="C5" s="1">
-        <v>1.3199290388658088E-22</v>
+        <v>844.07011832053126</v>
       </c>
       <c r="D5" s="1">
-        <v>72234525680115.578</v>
+        <v>0.9831993697443856</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>0.16302238727068941</v>
       </c>
       <c r="F5" s="1">
-        <v>39.340521412847934</v>
+        <v>-1615.0369104953934</v>
       </c>
       <c r="G5" s="1">
-        <v>39.340521412847934</v>
+        <v>1693.7179533210892</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -809,19 +809,19 @@
         <v>-740.53996141705261</v>
       </c>
       <c r="C6" s="1">
-        <v>3.8667858590829931E-19</v>
+        <v>19702.836261597535</v>
       </c>
       <c r="D6" s="1">
-        <v>-25121955602920.891</v>
+        <v>-0.79286593018176499</v>
       </c>
       <c r="E6" s="1">
-        <v>1</v>
+        <v>0.78586030175192978</v>
       </c>
       <c r="F6" s="1">
-        <v>-740.53996141705261</v>
+        <v>-39358.099034148217</v>
       </c>
       <c r="G6" s="1">
-        <v>-740.53996141705261</v>
+        <v>37877.019111314112</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -832,19 +832,19 @@
         <v>60.082333940137758</v>
       </c>
       <c r="C7" s="1">
-        <v>1.0018229864002514E-21</v>
+        <v>1121.4284432504242</v>
       </c>
       <c r="D7" s="1">
-        <v>40043433083228.328</v>
+        <v>1.130199818438733</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>0.12950110142460092</v>
       </c>
       <c r="F7" s="1">
-        <v>60.082333940137758</v>
+        <v>-2137.9174148306938</v>
       </c>
       <c r="G7" s="1">
-        <v>60.082333940137758</v>
+        <v>2258.0820827109692</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -855,19 +855,19 @@
         <v>-2.9857738816070206E-2</v>
       </c>
       <c r="C8" s="1">
-        <v>6.7646512313024711E-29</v>
+        <v>2.1627850076780422</v>
       </c>
       <c r="D8" s="1">
-        <v>-76579797743478.219</v>
+        <v>-0.29122159072364634</v>
       </c>
       <c r="E8" s="1">
-        <v>1</v>
+        <v>0.61449107639369227</v>
       </c>
       <c r="F8" s="1">
-        <v>-2.9857738816070206E-2</v>
+        <v>-4.2689163538650332</v>
       </c>
       <c r="G8" s="1">
-        <v>-2.9857738816070206E-2</v>
+        <v>4.2092008762328925</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -878,19 +878,19 @@
         <v>0.17535467119474774</v>
       </c>
       <c r="C9" s="1">
-        <v>-2.2911811286515877E-29</v>
+        <v>2.7490412838115899</v>
       </c>
       <c r="D9" s="1">
-        <v>772800924679432.25</v>
+        <v>1.3456003236602017</v>
       </c>
       <c r="E9" s="1">
-        <v>0</v>
+        <v>8.9559094438323328E-2</v>
       </c>
       <c r="F9" s="1">
-        <v>0.17535467119474774</v>
+        <v>-5.2127662450759686</v>
       </c>
       <c r="G9" s="1">
-        <v>0.17535467119474774</v>
+        <v>5.5634755874654633</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -901,19 +901,19 @@
         <v>1316.0319716818283</v>
       </c>
       <c r="C10" s="1">
-        <v>6.2012959760441762E-21</v>
+        <v>31408.597060780816</v>
       </c>
       <c r="D10" s="1">
-        <v>352537415003057.81</v>
+        <v>0.88388936322265055</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
+        <v>0.18861714753315151</v>
       </c>
       <c r="F10" s="1">
-        <v>1316.0319716818283</v>
+        <v>-60244.818267448572</v>
       </c>
       <c r="G10" s="1">
-        <v>1316.0319716818283</v>
+        <v>62876.882210812226</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -924,19 +924,19 @@
         <v>-1167.6884001688611</v>
       </c>
       <c r="C11" s="1">
-        <v>1.8510307821365774E-21</v>
+        <v>26600.901698513204</v>
       </c>
       <c r="D11" s="1">
-        <v>-572532508362519.88</v>
+        <v>-0.92599920354960619</v>
       </c>
       <c r="E11" s="1">
-        <v>1</v>
+        <v>0.82252528389353907</v>
       </c>
       <c r="F11" s="1">
-        <v>-1167.6884001688611</v>
+        <v>-53305.45572925474</v>
       </c>
       <c r="G11" s="1">
-        <v>-1167.6884001688611</v>
+        <v>50970.078928917021</v>
       </c>
     </row>
   </sheetData>

</xml_diff>